<commit_message>
extract environment constants in django server out and put them into docker-compose.yml, update my timesheet
</commit_message>
<xml_diff>
--- a/Time sheet/Timetsheet - Ka Yiu Eric Ma.xlsx
+++ b/Time sheet/Timetsheet - Ka Yiu Eric Ma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Google Drive/U Adelaide course materials/MCI projects/Team-024/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CE099A-BC7F-0049-BD8C-6B221F1FB5AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401D875B-A01D-7D40-8341-F0A1D515CF72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="4" r:id="rId1"/>
@@ -18,17 +18,26 @@
     <sheet name="Week 3" sheetId="1" r:id="rId3"/>
     <sheet name="Week 4" sheetId="5" r:id="rId4"/>
     <sheet name="Week 5" sheetId="6" r:id="rId5"/>
+    <sheet name="Week 6" sheetId="8" r:id="rId6"/>
+    <sheet name="Sem Break Week 1" sheetId="9" r:id="rId7"/>
+    <sheet name="Sem Break Week 2" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Sem Break Week 1'!$A$1:$H$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'Sem Break Week 2'!$A$1:$H$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 1'!$A$1:$H$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Week 2'!$A$1:$H$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Week 3'!$A$1:$H$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Week 4'!$A$1:$H$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Week 5'!$A$1:$H$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Week 6'!$A$1:$H$13</definedName>
+    <definedName name="Week_Start" localSheetId="6">'Sem Break Week 1'!$C$4</definedName>
+    <definedName name="Week_Start" localSheetId="7">'Sem Break Week 2'!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="0">'Week 1'!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="1">'Week 2'!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="3">'Week 4'!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="4">'Week 5'!$C$4</definedName>
+    <definedName name="Week_Start" localSheetId="5">'Week 6'!$C$4</definedName>
     <definedName name="Week_Start">'Week 3'!$C$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -50,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="74">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -194,6 +203,84 @@
   </si>
   <si>
     <t>Complete the 'What', 'Why', 'Roles and Permissions' of the business case, first milestone plan draft</t>
+  </si>
+  <si>
+    <t>Complete 70% of the online course at Udemy</t>
+  </si>
+  <si>
+    <t>Learn Docker and Django server, Django Rest Framework for backend development</t>
+  </si>
+  <si>
+    <t>Complete 10% of the online course for Docker and Django at Udemy</t>
+  </si>
+  <si>
+    <t>Complete 20% of the online course for Docker and Django at Udemy</t>
+  </si>
+  <si>
+    <t>Complete 30% of the online course for Docker and Django at Udemy</t>
+  </si>
+  <si>
+    <t>Semester Break Week 1</t>
+  </si>
+  <si>
+    <t>Semester Break Week 2</t>
+  </si>
+  <si>
+    <t>Complete 40% of the online course for Docker and Django at Udemy</t>
+  </si>
+  <si>
+    <t>Complete 50% of the online course for Docker and Django at Udemy</t>
+  </si>
+  <si>
+    <t>Complete 60% of the online course for Docker and Django at Udemy</t>
+  </si>
+  <si>
+    <t>Complete 70% of the online course for Docker and Django at Udemy</t>
+  </si>
+  <si>
+    <t>For implementation of user authentication and home page features. They are tasks listed on the project plan .</t>
+  </si>
+  <si>
+    <t>Created the docker file and docker-compose.yml that will install project dependencies; Create Django project; Fix bugs in home page reported by team mates</t>
+  </si>
+  <si>
+    <t>Set up Docker container and Django server for Mindspace. Fix bugs in home page.</t>
+  </si>
+  <si>
+    <t>Fix the bug and will pass the work to Jason for complete the remaining implementation</t>
+  </si>
+  <si>
+    <t>Complete 80% of the online course for Docker and Django at Udemy</t>
+  </si>
+  <si>
+    <t>Fix problems in getting mysql server to run in the Docker Container</t>
+  </si>
+  <si>
+    <t>For implementation of user authentication, which is a task listed on the milestone 1 plan.</t>
+  </si>
+  <si>
+    <t>For implementation of home page features, which is a task listed on the milestone 1 plan.</t>
+  </si>
+  <si>
+    <t>Fix all the problems related to getting mysql to run with Django server in the Docker container</t>
+  </si>
+  <si>
+    <t>Complete the functionality of /api/user/token/ in Django server. Update ionic app to complete user authentication workflow.</t>
+  </si>
+  <si>
+    <t>Implement the endpoint of Django server for validating FireAuth token and exchanging tokens for authentication in Django Server. Update ionic app to process user authentication</t>
+  </si>
+  <si>
+    <t>For implementation of user authentication and home page features, which are tasks listed on the milestone 1 plan.</t>
+  </si>
+  <si>
+    <t>Complete the functionality of /api/record/emotions/ in Django server. Update ionic app to allow loading sample data from the Django server.</t>
+  </si>
+  <si>
+    <t>Implement loading sample data provided by clients into mysql database of the Django server. Implement the endpoint of Django server for loading sample data. Update ionic app to allow making http request to load sample data from the Django server</t>
+  </si>
+  <si>
+    <t>Fix bug in home page that the http request of loading sample data triggers only once</t>
   </si>
 </sst>
 </file>
@@ -341,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -397,9 +484,6 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -417,6 +501,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -763,8 +853,8 @@
   </sheetPr>
   <dimension ref="A2:AW12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,16 +870,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1227,7 +1317,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1243,16 +1333,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1734,16 +1824,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1804,19 +1894,19 @@
       <c r="B6" s="20">
         <v>44270</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>0.375</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>0.625</v>
       </c>
       <c r="E6" s="12">
         <v>6</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="10" t="s">
@@ -1869,11 +1959,11 @@
         <v>13</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="10"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
@@ -1924,22 +2014,22 @@
       <c r="B8" s="20">
         <v>44272</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>0.375</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <v>0.75</v>
       </c>
       <c r="E8" s="12">
         <v>9</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>31</v>
       </c>
       <c r="I8" s="13"/>
@@ -1991,19 +2081,19 @@
       <c r="B9" s="20">
         <v>44273</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <v>0.875</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>0.625</v>
       </c>
       <c r="E9" s="12">
         <v>6</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="10" t="s">
@@ -2217,16 +2307,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2281,25 +2371,25 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:49" s="14" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="20">
         <v>44277</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>0.375</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>0.5</v>
       </c>
       <c r="E6" s="12">
         <v>3</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="10" t="s">
@@ -2352,12 +2442,12 @@
         <v>13</v>
       </c>
       <c r="B7" s="20"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="25"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
@@ -2401,28 +2491,28 @@
       <c r="AW7" s="13"/>
     </row>
     <row r="8" spans="1:49" s="14" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="20">
         <v>44279</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="21">
         <v>0.375</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="21">
         <v>0.75</v>
       </c>
       <c r="E8" s="12">
         <v>9</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>31</v>
       </c>
       <c r="I8" s="13"/>
@@ -2474,22 +2564,22 @@
       <c r="B9" s="20">
         <v>44280</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <v>0.625</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>0.75</v>
       </c>
       <c r="E9" s="12">
         <v>3</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>37</v>
       </c>
       <c r="I9" s="13"/>
@@ -2535,25 +2625,25 @@
       <c r="AW9" s="13"/>
     </row>
     <row r="10" spans="1:49" s="14" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="20">
         <v>44281</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="21">
         <v>0.875</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="21">
         <v>0.625</v>
       </c>
       <c r="E10" s="12">
         <v>6</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="22" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="10" t="s">
@@ -2606,11 +2696,11 @@
         <v>17</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="10"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
@@ -2692,7 +2782,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2708,16 +2798,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2772,25 +2862,25 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:49" s="14" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="20">
         <v>44284</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>0.375</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>0.625</v>
       </c>
       <c r="E6" s="12">
         <v>6</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>40</v>
       </c>
       <c r="H6" s="10" t="s">
@@ -2845,22 +2935,22 @@
       <c r="B7" s="20">
         <v>44285</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <v>0.875</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>0.75</v>
       </c>
       <c r="E7" s="12">
         <v>9</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>44</v>
       </c>
       <c r="I7" s="13"/>
@@ -2906,25 +2996,25 @@
       <c r="AW7" s="13"/>
     </row>
     <row r="8" spans="1:49" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="20">
         <v>44286</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>0.625</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <v>0.75</v>
       </c>
       <c r="E8" s="12">
         <v>3</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="22" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="10" t="s">
@@ -2979,22 +3069,22 @@
       <c r="B9" s="20">
         <v>44287</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <v>0.5</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>0.75</v>
       </c>
       <c r="E9" s="12">
         <v>6</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>47</v>
       </c>
       <c r="I9" s="13"/>
@@ -3040,15 +3130,15 @@
       <c r="AW9" s="13"/>
     </row>
     <row r="10" spans="1:49" s="14" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="10"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -3097,11 +3187,11 @@
         <v>17</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="10"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
@@ -3173,4 +3263,1505 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF20900-60AB-CF4A-8782-F9F03233C2AF}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AW12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="15" max="49" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1792052</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:49" s="14" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="20">
+        <v>44291</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="E6" s="12">
+        <v>6</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+    </row>
+    <row r="7" spans="1:49" s="14" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+    </row>
+    <row r="8" spans="1:49" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="20">
+        <v>44293</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="E8" s="12">
+        <v>6</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="13"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+      <c r="AW8" s="13"/>
+    </row>
+    <row r="9" spans="1:49" s="14" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="20">
+        <v>44294</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="E9" s="12">
+        <v>6</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+      <c r="AN9" s="13"/>
+      <c r="AO9" s="13"/>
+      <c r="AP9" s="13"/>
+      <c r="AQ9" s="13"/>
+      <c r="AR9" s="13"/>
+      <c r="AS9" s="13"/>
+      <c r="AT9" s="13"/>
+      <c r="AU9" s="13"/>
+      <c r="AV9" s="13"/>
+      <c r="AW9" s="13"/>
+    </row>
+    <row r="10" spans="1:49" s="14" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="20">
+        <v>44295</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="E10" s="12">
+        <v>6</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="13"/>
+      <c r="AP10" s="13"/>
+      <c r="AQ10" s="13"/>
+      <c r="AR10" s="13"/>
+      <c r="AS10" s="13"/>
+      <c r="AT10" s="13"/>
+      <c r="AU10" s="13"/>
+      <c r="AV10" s="13"/>
+      <c r="AW10" s="13"/>
+    </row>
+    <row r="11" spans="1:49" s="14" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+      <c r="AN11" s="13"/>
+      <c r="AO11" s="13"/>
+      <c r="AP11" s="13"/>
+      <c r="AQ11" s="13"/>
+      <c r="AR11" s="13"/>
+      <c r="AS11" s="13"/>
+      <c r="AT11" s="13"/>
+      <c r="AU11" s="13"/>
+      <c r="AV11" s="13"/>
+      <c r="AW11" s="13"/>
+    </row>
+    <row r="12" spans="1:49" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8">
+        <f>SUM(E6:E11)</f>
+        <v>24</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D11" xr:uid="{668CC58F-D24C-3644-AE65-21B358022D07}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC1516B-30DD-CC45-A670-14140C5EFD35}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AW12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="15" max="49" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1792052</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:49" s="14" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="20">
+        <v>44298</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="E6" s="12">
+        <v>9</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+    </row>
+    <row r="7" spans="1:49" s="14" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="20">
+        <v>44299</v>
+      </c>
+      <c r="C7" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D7" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="12">
+        <v>9</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+    </row>
+    <row r="8" spans="1:49" s="14" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="20">
+        <v>44300</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="12">
+        <v>9</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="13"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+      <c r="AW8" s="13"/>
+    </row>
+    <row r="9" spans="1:49" s="14" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="20">
+        <v>44301</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D9" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="12">
+        <v>4</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+      <c r="AN9" s="13"/>
+      <c r="AO9" s="13"/>
+      <c r="AP9" s="13"/>
+      <c r="AQ9" s="13"/>
+      <c r="AR9" s="13"/>
+      <c r="AS9" s="13"/>
+      <c r="AT9" s="13"/>
+      <c r="AU9" s="13"/>
+      <c r="AV9" s="13"/>
+      <c r="AW9" s="13"/>
+    </row>
+    <row r="10" spans="1:49" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="20">
+        <v>44302</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E10" s="12">
+        <v>9</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="13"/>
+      <c r="AP10" s="13"/>
+      <c r="AQ10" s="13"/>
+      <c r="AR10" s="13"/>
+      <c r="AS10" s="13"/>
+      <c r="AT10" s="13"/>
+      <c r="AU10" s="13"/>
+      <c r="AV10" s="13"/>
+      <c r="AW10" s="13"/>
+    </row>
+    <row r="11" spans="1:49" s="14" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+      <c r="AN11" s="13"/>
+      <c r="AO11" s="13"/>
+      <c r="AP11" s="13"/>
+      <c r="AQ11" s="13"/>
+      <c r="AR11" s="13"/>
+      <c r="AS11" s="13"/>
+      <c r="AT11" s="13"/>
+      <c r="AU11" s="13"/>
+      <c r="AV11" s="13"/>
+      <c r="AW11" s="13"/>
+    </row>
+    <row r="12" spans="1:49" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8">
+        <f>SUM(E6:E11)</f>
+        <v>40</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D11" xr:uid="{1A18F25C-C319-8641-BFDE-A09C468FEF53}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75175FFF-FD73-8342-B6F9-91B7A0AFDA89}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AW12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="15" max="49" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1792052</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:49" s="14" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="20">
+        <v>44305</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="E6" s="12">
+        <v>6</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+    </row>
+    <row r="7" spans="1:49" s="14" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="20">
+        <v>44306</v>
+      </c>
+      <c r="C7" s="21">
+        <v>0.875</v>
+      </c>
+      <c r="D7" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="12">
+        <v>9</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+    </row>
+    <row r="8" spans="1:49" s="14" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="20">
+        <v>44307</v>
+      </c>
+      <c r="C8" s="21">
+        <v>0.875</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="12">
+        <v>9</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="13"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+      <c r="AW8" s="13"/>
+    </row>
+    <row r="9" spans="1:49" s="14" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="20">
+        <v>44308</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0.875</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="12">
+        <v>9</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+      <c r="AN9" s="13"/>
+      <c r="AO9" s="13"/>
+      <c r="AP9" s="13"/>
+      <c r="AQ9" s="13"/>
+      <c r="AR9" s="13"/>
+      <c r="AS9" s="13"/>
+      <c r="AT9" s="13"/>
+      <c r="AU9" s="13"/>
+      <c r="AV9" s="13"/>
+      <c r="AW9" s="13"/>
+    </row>
+    <row r="10" spans="1:49" s="14" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="20">
+        <v>44309</v>
+      </c>
+      <c r="C10" s="21">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E10" s="12">
+        <v>2</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="13"/>
+      <c r="AP10" s="13"/>
+      <c r="AQ10" s="13"/>
+      <c r="AR10" s="13"/>
+      <c r="AS10" s="13"/>
+      <c r="AT10" s="13"/>
+      <c r="AU10" s="13"/>
+      <c r="AV10" s="13"/>
+      <c r="AW10" s="13"/>
+    </row>
+    <row r="11" spans="1:49" s="14" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+      <c r="AN11" s="13"/>
+      <c r="AO11" s="13"/>
+      <c r="AP11" s="13"/>
+      <c r="AQ11" s="13"/>
+      <c r="AR11" s="13"/>
+      <c r="AS11" s="13"/>
+      <c r="AT11" s="13"/>
+      <c r="AU11" s="13"/>
+      <c r="AV11" s="13"/>
+      <c r="AW11" s="13"/>
+    </row>
+    <row r="12" spans="1:49" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8">
+        <f>SUM(E6:E11)</f>
+        <v>35</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D11" xr:uid="{556E6B0B-02B6-F84B-94A0-C42DB2449953}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>